<commit_message>
The course and its related control logic have been added, and now students and their points are dependent on the course.
</commit_message>
<xml_diff>
--- a/test_students.xlsx
+++ b/test_students.xlsx
@@ -1,46 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29515"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Software_Engineering_Practice\3_cowork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3B70DF-564C-48DF-8199-C13CC0AB870E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="学生名单" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>学号</t>
+  </si>
+  <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>专业</t>
+  </si>
+  <si>
+    <t>2021001</t>
+  </si>
+  <si>
+    <t>张三</t>
+  </si>
+  <si>
+    <t>计算机科学</t>
+  </si>
+  <si>
+    <t>2021002</t>
+  </si>
+  <si>
+    <t>李四</t>
+  </si>
+  <si>
+    <t>信息工程</t>
+  </si>
+  <si>
+    <t>2021003</t>
+  </si>
+  <si>
+    <t>软件工程</t>
+  </si>
+  <si>
+    <t>2021004</t>
+  </si>
+  <si>
+    <t>王五</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王六</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -65,13 +107,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,169 +446,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>学号</v>
-      </c>
-      <c r="B1" t="str">
-        <v>姓名</v>
-      </c>
-      <c r="C1" t="str">
-        <v>专业</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>2021001</v>
-      </c>
-      <c r="B2" t="str">
-        <v>张三</v>
-      </c>
-      <c r="C2" t="str">
-        <v>计算机科学</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2021002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>李四</v>
-      </c>
-      <c r="C3" t="str">
-        <v>信息工程</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2021003</v>
-      </c>
-      <c r="B4" t="str">
-        <v>王五</v>
-      </c>
-      <c r="C4" t="str">
-        <v>软件工程</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2021004</v>
-      </c>
-      <c r="B5" t="str">
-        <v>赵六</v>
-      </c>
-      <c r="C5" t="str">
-        <v>计算机科学</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2021005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>孙七</v>
-      </c>
-      <c r="C6" t="str">
-        <v>信息工程</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>2021006</v>
-      </c>
-      <c r="B7" t="str">
-        <v>周八</v>
-      </c>
-      <c r="C7" t="str">
-        <v>软件工程</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>2021007</v>
-      </c>
-      <c r="B8" t="str">
-        <v>吴九</v>
-      </c>
-      <c r="C8" t="str">
-        <v>计算机科学</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>2021008</v>
-      </c>
-      <c r="B9" t="str">
-        <v>郑十</v>
-      </c>
-      <c r="C9" t="str">
-        <v>信息工程</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>2021009</v>
-      </c>
-      <c r="B10" t="str">
-        <v>王十一</v>
-      </c>
-      <c r="C10" t="str">
-        <v>软件工程</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>2021010</v>
-      </c>
-      <c r="B11" t="str">
-        <v>陈十二</v>
-      </c>
-      <c r="C11" t="str">
-        <v>计算机科学</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>2021011</v>
-      </c>
-      <c r="B12" t="str">
-        <v>林十三</v>
-      </c>
-      <c r="C12" t="str">
-        <v>信息工程</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>2021012</v>
-      </c>
-      <c r="B13" t="str">
-        <v>黄十四</v>
-      </c>
-      <c r="C13" t="str">
-        <v>软件工程</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>2021013</v>
-      </c>
-      <c r="B14" t="str">
-        <v>徐十五</v>
-      </c>
-      <c r="C14" t="str">
-        <v>计算机科学</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C14"/>
+    <ignoredError sqref="A1:C3 A4 C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>